<commit_message>
Update MaxDuino Development Roadmap.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/MaxDuino Development Roadmap.xlsx
+++ b/Documentation/MaxDuino Development Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Alan\Arduino\Arduino Sketches\GitHub\MaxDuino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD525EC4-FFFC-44F6-86D8-49B1B600ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40B7D60-952B-405B-932E-756665B43ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B16E0DF9-CE6E-473D-A853-270CC3AD2790}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t>Section</t>
   </si>
@@ -116,9 +116,6 @@
     <t>DCC Decode</t>
   </si>
   <si>
-    <t>2 layer Through Hole PCB</t>
-  </si>
-  <si>
     <t>Flexible</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Year</t>
   </si>
   <si>
     <t>Add SPI (Header) to MaxDuino</t>
@@ -424,6 +418,15 @@
   <si>
     <t>Weigh pros and cons carefully before proceeding. 
 ESP32 module or native chip?</t>
+  </si>
+  <si>
+    <t>2 layer TH PCB</t>
+  </si>
+  <si>
+    <t>5YP Planning Year</t>
+  </si>
+  <si>
+    <t>Calendar Year</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +484,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -551,7 +561,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -563,21 +573,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -728,12 +723,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -762,66 +892,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,79 +941,91 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -934,36 +1053,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1286,7 +1375,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,72 +1387,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="A1" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>51</v>
+      <c r="A2" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,14 +1464,14 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D6">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"In Progress"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Defer"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"New"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"Defer"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,21 +1496,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B95C216-D2B5-4291-A214-83500FF62971}">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="24" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.5703125" customWidth="1"/>
+    <col min="16" max="24" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1429,180 +1520,182 @@
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="63">
+        <v>40</v>
+      </c>
+      <c r="E1" s="55">
         <v>1</v>
       </c>
-      <c r="F1" s="26">
+      <c r="F1" s="56">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="64">
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59">
         <v>1.2</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="39">
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="62">
         <v>2</v>
       </c>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="40"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="63"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="46">
+      <c r="B2" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="67">
         <v>1</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="57">
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69">
         <v>2</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="46">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="68">
         <v>3</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="57">
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="69">
         <v>4</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="46">
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="68">
         <v>5</v>
       </c>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="48"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="70"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="49">
+      <c r="B3" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="71">
         <v>2023</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="51"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="54">
         <v>2024</v>
       </c>
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
       <c r="L3" s="54"/>
-      <c r="M3" s="49">
+      <c r="M3" s="53">
         <v>2025</v>
       </c>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="51"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
       <c r="Q3" s="54">
         <v>2026</v>
       </c>
       <c r="R3" s="54"/>
       <c r="S3" s="54"/>
       <c r="T3" s="54"/>
-      <c r="U3" s="49">
+      <c r="U3" s="53">
         <v>2027</v>
       </c>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="51"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="72"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="22" t="s">
+      <c r="S4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="T4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="U4" s="25" t="s">
+      <c r="U4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="22" t="s">
+      <c r="W4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="24" t="s">
+      <c r="X4" s="76" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1612,374 +1705,374 @@
         <v>7</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="74"/>
+        <v>112</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="43"/>
     </row>
     <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="76"/>
-      <c r="W6" s="76"/>
-      <c r="X6" s="77"/>
+        <v>16</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
+      <c r="X6" s="43"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="62"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="76" t="s">
-        <v>112</v>
-      </c>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="76"/>
-      <c r="W7" s="76"/>
-      <c r="X7" s="77"/>
+        <v>17</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="43"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="76"/>
-      <c r="X8" s="77"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="43"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="77"/>
+        <v>18</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="43"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="77"/>
+        <v>18</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="43"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="30" t="s">
-        <v>68</v>
+        <v>19</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="22" t="s">
+        <v>66</v>
       </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76"/>
-      <c r="S11" s="76"/>
-      <c r="T11" s="76"/>
-      <c r="U11" s="78"/>
-      <c r="V11" s="76"/>
-      <c r="W11" s="76"/>
-      <c r="X11" s="77"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="43"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="85"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="76"/>
-      <c r="S12" s="76"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="78"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="76"/>
-      <c r="X12" s="77"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="43"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="76"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="76"/>
-      <c r="X13" s="77"/>
+        <v>18</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="43"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="16" t="s">
-        <v>28</v>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="29"/>
+        <v>29</v>
+      </c>
+      <c r="E14" s="21"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="30" t="s">
-        <v>67</v>
+      <c r="G14" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="76"/>
-      <c r="R14" s="76"/>
-      <c r="S14" s="76"/>
-      <c r="T14" s="76"/>
-      <c r="U14" s="78"/>
-      <c r="V14" s="76"/>
-      <c r="W14" s="76"/>
-      <c r="X14" s="77"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
+      <c r="X14" s="43"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="71"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="81"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="80"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="U2:X2"/>
     <mergeCell ref="E3:H3"/>
-    <mergeCell ref="B3:D3"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="U3:X3"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2005,33 +2098,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="34"/>
+      <c r="A1" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>78</v>
+      <c r="A2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2039,17 +2132,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="44" t="s">
-        <v>32</v>
+      <c r="C3" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2057,17 +2150,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="44" t="s">
-        <v>33</v>
+      <c r="C4" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2075,35 +2168,35 @@
         <v>3</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="44" t="s">
-        <v>94</v>
+      <c r="C5" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="44" t="s">
-        <v>43</v>
+      <c r="B6" s="42"/>
+      <c r="C6" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2213,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,105 +2232,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59" t="s">
-        <v>50</v>
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="34" t="s">
+      <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>38</v>
+      <c r="B4" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="K4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="34">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
-        <v>2</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="45">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2286,85 +2379,85 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="F3" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="F5" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="37"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>